<commit_message>
fix summary average value
</commit_message>
<xml_diff>
--- a/App/LCFC-ScoutingApp/back-end/Report.xlsx
+++ b/App/LCFC-ScoutingApp/back-end/Report.xlsx
@@ -16,7 +16,7 @@
     <t>Fixture</t>
   </si>
   <si>
-    <t>Atletico Madrid vs Liverpool</t>
+    <t>Chelsea vs Arsenal</t>
   </si>
   <si>
     <t>Striker</t>
@@ -25,13 +25,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Diego Costa</t>
+    <t>Sean Raisi</t>
   </si>
   <si>
     <t>Height</t>
   </si>
   <si>
-    <t>6.1</t>
+    <t>5.7</t>
   </si>
   <si>
     <t>Position</t>
@@ -40,36 +40,39 @@
     <t>Playing Against</t>
   </si>
   <si>
-    <t>Liverpool</t>
+    <t>Arsenal</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>12/03/2020</t>
+    <t>22/01/18</t>
   </si>
   <si>
     <t>Age</t>
   </si>
   <si>
-    <t>30</t>
+    <t>19</t>
   </si>
   <si>
     <t>Club</t>
   </si>
   <si>
-    <t>Atletico Madrid</t>
+    <t>Chelsea</t>
   </si>
   <si>
     <t>H/T</t>
   </si>
   <si>
-    <t>0-1</t>
+    <t>2-0</t>
   </si>
   <si>
     <t>F/T</t>
   </si>
   <si>
+    <t>3-0</t>
+  </si>
+  <si>
     <t>Scout</t>
   </si>
   <si>
@@ -82,7 +85,7 @@
     <t>Hold Up Play</t>
   </si>
   <si>
-    <t>5</t>
+    <t>9</t>
   </si>
   <si>
     <t>Receiving Under Pressure</t>
@@ -145,70 +148,67 @@
     <t>Runs Off The Shoulder</t>
   </si>
   <si>
+    <t>Running The Channels</t>
+  </si>
+  <si>
+    <t>Movement Off The Ball</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Pace</t>
+  </si>
+  <si>
+    <t>Mobility</t>
+  </si>
+  <si>
+    <t>Stength/Planning</t>
+  </si>
+  <si>
+    <t>Work Rate</t>
+  </si>
+  <si>
+    <t>Jump/Spring</t>
+  </si>
+  <si>
+    <t>Psychological</t>
+  </si>
+  <si>
+    <t>Bravery</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>Team Work</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Response To Criticsm</t>
+  </si>
+  <si>
+    <t>Reaction To Mistakes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Running The Channels</t>
-  </si>
-  <si>
-    <t>Movement Off The Ball</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>Pace</t>
-  </si>
-  <si>
-    <t>Mobility</t>
-  </si>
-  <si>
-    <t>Stength/Planning</t>
-  </si>
-  <si>
-    <t>Work Rate</t>
-  </si>
-  <si>
-    <t>Jump/Spring</t>
-  </si>
-  <si>
-    <t>Psychological</t>
-  </si>
-  <si>
-    <t>Bravery</t>
-  </si>
-  <si>
-    <t>Leadership</t>
-  </si>
-  <si>
-    <t>Team Work</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>Response To Criticsm</t>
-  </si>
-  <si>
-    <t>Reaction To Mistakes</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Nasty</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
-    <t>Costa, Diego was scouted playing for Atletico Madrid on 12/03/2020. Costa, Diego performed to grade B with an average score of 0 showing some outstanding attributes, hold up play (5), receiving under pressure (5), link up play (5), right foot (5), left foot (5), one v one (5), aerial ability (5), finishing (5), right foot shooting (5), left foot shooting (5), crossing (5), one v two (5), tackling (5), pressing (5), recovering into shape (5), agility (5), dropping into space (5), jump (5).</t>
+    <t>Raisi, Sean was scouted playing for Chelsea on 22/01/18. Raisi, Sean performed to grade A with an average score of 9 showing some outstanding attributes.</t>
   </si>
   <si>
     <t>Player Rating</t>
   </si>
   <si>
-    <t>B</t>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -348,7 +348,7 @@
       </c>
       <c r="K7" s="0"/>
       <c r="L7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M7" s="0"/>
     </row>
@@ -365,32 +365,32 @@
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
       <c r="N8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O8" s="0"/>
       <c r="P8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="0"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
       <c r="D12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H12" s="0"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K12" s="0"/>
       <c r="L12" s="0"/>
@@ -407,231 +407,231 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="0"/>
       <c r="F13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K13" s="0"/>
       <c r="L13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>48</v>
       </c>
       <c r="N13" s="0"/>
       <c r="O13" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P13" s="0" t="s">
         <v>54</v>
       </c>
       <c r="Q13" s="0"/>
       <c r="R13" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" s="0"/>
       <c r="F14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H14" s="0"/>
       <c r="I14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K14" s="0"/>
       <c r="L14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M14" s="0" t="s">
         <v>49</v>
       </c>
       <c r="N14" s="0"/>
       <c r="O14" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P14" s="0" t="s">
         <v>55</v>
       </c>
       <c r="Q14" s="0"/>
       <c r="R14" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" s="0"/>
       <c r="F15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K15" s="0"/>
       <c r="L15" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>50</v>
       </c>
       <c r="N15" s="0"/>
       <c r="O15" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P15" s="0" t="s">
         <v>56</v>
       </c>
       <c r="Q15" s="0"/>
       <c r="R15" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>45</v>
       </c>
       <c r="K16" s="0"/>
       <c r="L16" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="M16" s="0" t="s">
         <v>51</v>
       </c>
       <c r="N16" s="0"/>
       <c r="O16" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P16" s="0" t="s">
         <v>57</v>
       </c>
       <c r="Q16" s="0"/>
       <c r="R16" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" s="0"/>
       <c r="F17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>46</v>
       </c>
       <c r="K17" s="0"/>
       <c r="L17" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="M17" s="0" t="s">
         <v>52</v>
       </c>
       <c r="N17" s="0"/>
       <c r="O17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P17" s="0" t="s">
         <v>58</v>
       </c>
       <c r="Q17" s="0"/>
       <c r="R17" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="4:18">
       <c r="D18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18" s="0"/>
       <c r="F18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P18" s="0" t="s">
         <v>59</v>
       </c>
       <c r="Q18" s="0"/>
       <c r="R18" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:18">

</xml_diff>